<commit_message>
Adding download rollouts automatically.
</commit_message>
<xml_diff>
--- a/data/Extensions.xlsx
+++ b/data/Extensions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gxologistics-my.sharepoint.com/personal/xavier_parro_gxo_com/Documents/1. GXO/3. Internal/3. Developments/2. BY Instances Manager/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="8_{3A3C676D-04FE-46A3-BA85-E52D00AEE8F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D496C2ED-E039-4E38-AC1F-03B8E8A50F69}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="8_{3A3C676D-04FE-46A3-BA85-E52D00AEE8F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E616890A-D1E5-4B42-91BB-7AE0D58D22A4}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="816" windowWidth="23256" windowHeight="13896" xr2:uid="{3AFE9030-45BA-40A4-AA93-EF8467272483}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Instance</t>
   </si>
@@ -64,9 +64,6 @@
     <t>PRD</t>
   </si>
   <si>
-    <t>CT_REPORT_00303_V.001.ta</t>
-  </si>
-  <si>
     <t>KUMHO Packing List</t>
   </si>
   <si>
@@ -74,6 +71,27 @@
   </si>
   <si>
     <t>NO</t>
+  </si>
+  <si>
+    <t>RG_PAGEBUILDER_00052_V.003</t>
+  </si>
+  <si>
+    <t>CT_REPORT_00303_V.001.tar</t>
+  </si>
+  <si>
+    <t>PB to create Orders</t>
+  </si>
+  <si>
+    <t>PR10</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>KUMHO - 3036</t>
+  </si>
+  <si>
+    <t>Soda Stream</t>
   </si>
 </sst>
 </file>
@@ -117,7 +135,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -128,7 +146,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -466,28 +483,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11A76667-0CAD-4F16-B578-156EFED1F1DC}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G2"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.6328125" customWidth="1"/>
     <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.6328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.6328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.6328125" customWidth="1"/>
-    <col min="10" max="10" width="54.1796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="54.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.54296875" customWidth="1"/>
+    <col min="4" max="4" width="8.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.6328125" customWidth="1"/>
+    <col min="11" max="11" width="54.1796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="54.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -495,52 +513,71 @@
         <v>3</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="F2" s="4">
+        <v>45666</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="5">
-        <v>45666</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -548,6 +585,7 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>